<commit_message>
Replaced refund report with latest report
</commit_message>
<xml_diff>
--- a/public/files/refund-report.xlsx
+++ b/public/files/refund-report.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JaimeLHabersat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSA Data\Reports\Refund Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56B669C-97F0-43E5-9512-84E5027E9F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AC2405-6001-4E38-AEDB-2BA0A1F207E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{59F6B7B8-CB1F-4012-B8AB-951C4865ED6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{59F6B7B8-CB1F-4012-B8AB-951C4865ED6A}"/>
   </bookViews>
   <sheets>
-    <sheet name="GSA SmartPay Net Refunds" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="GSA SmartPay Net Refunds Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="GSA SmartPay Net Refunds" sheetId="1" r:id="rId1"/>
+    <sheet name="GSA SmartPay Net Refunds Chart" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>09</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25*</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>FY25 is through 3/31/2025.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -160,12 +172,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -226,7 +239,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="1"/>
-              <a:t>GSA SmartPay Net Refunds</a:t>
+              <a:t>GSA SmartPay(R) Net Refunds</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -293,7 +306,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
             <a:ln w="111125">
               <a:solidFill>
@@ -312,7 +325,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -338,7 +351,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -364,7 +377,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -390,7 +403,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -416,7 +429,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -442,7 +455,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -468,7 +481,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -494,7 +507,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -520,7 +533,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -546,7 +559,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -572,7 +585,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -598,7 +611,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -624,7 +637,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -648,7 +661,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -672,7 +685,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -696,7 +709,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -720,7 +733,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -744,7 +757,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -768,7 +781,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -792,7 +805,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -816,7 +829,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -840,7 +853,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -864,7 +877,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -891,7 +904,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -918,7 +931,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -972,10 +985,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -993,6 +1003,60 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000034-4997-45EA-ACF8-DAC8DB9AF015}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="111125">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000036-01FC-4C42-9561-839368366CD4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="111125">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-01FC-4C42-9561-839368366CD4}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1020,7 +1084,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1069,7 +1133,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1118,7 +1182,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1167,7 +1231,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1208,7 +1272,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -1250,9 +1314,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'GSA SmartPay Net Refunds'!$A$4:$A$30</c:f>
+              <c:f>'GSA SmartPay Net Refunds'!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>97</c:v>
                 </c:pt>
@@ -1333,16 +1397,22 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>25*</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'GSA SmartPay Net Refunds'!$B$4:$B$30</c:f>
+              <c:f>'GSA SmartPay Net Refunds'!$B$4:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>6000000</c:v>
                 </c:pt>
@@ -1423,6 +1493,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>471856109.18874192</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>505920158.7602604</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>219609763.67566624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1461,7 +1537,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1493,7 +1569,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1531,7 +1607,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1567,7 +1643,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1580,7 +1656,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Dollars </a:t>
                 </a:r>
               </a:p>
@@ -1599,7 +1675,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1631,7 +1707,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4739,7 +4815,7 @@
       <cdr:y>0.89885</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38472</cdr:x>
+      <cdr:x>0.39841</cdr:x>
       <cdr:y>0.94336</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -4755,8 +4831,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2114551" y="4232138"/>
-          <a:ext cx="828675" cy="209550"/>
+          <a:off x="2114567" y="4232135"/>
+          <a:ext cx="933433" cy="209553"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4767,7 +4843,7 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>SmartPay</a:t>
           </a:r>
           <a:r>
@@ -4785,8 +4861,8 @@
       <cdr:y>0.89686</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.64534</cdr:x>
-      <cdr:y>0.94136</cdr:y>
+      <cdr:x>0.65115</cdr:x>
+      <cdr:y>0.95954</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4801,8 +4877,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4108450" y="4222750"/>
-          <a:ext cx="828675" cy="209550"/>
+          <a:off x="4108412" y="4222765"/>
+          <a:ext cx="873164" cy="295123"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4877,11 +4953,11 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>SmartPay</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
             <a:t> 2</a:t>
           </a:r>
         </a:p>
@@ -4894,8 +4970,8 @@
       <cdr:y>0.89686</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.86198</cdr:x>
-      <cdr:y>0.94136</cdr:y>
+      <cdr:x>0.88148</cdr:x>
+      <cdr:y>0.95145</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4910,8 +4986,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5765800" y="4222750"/>
-          <a:ext cx="828675" cy="209550"/>
+          <a:off x="5765793" y="4222765"/>
+          <a:ext cx="977908" cy="257023"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4986,7 +5062,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>SmartPay</a:t>
           </a:r>
           <a:r>
@@ -6012,19 +6088,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F221688A-C4CC-471D-9445-3D65F494C309}">
   <dimension ref="A1:AN45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
+      <c r="A1" s="7"/>
       <c r="B1" s="2"/>
       <c r="C1" s="5"/>
       <c r="D1" s="4"/>
@@ -6066,7 +6142,7 @@
       <c r="AN1" s="4"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2"/>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
@@ -6108,7 +6184,7 @@
       <c r="AN2" s="4"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -6154,7 +6230,7 @@
       <c r="AN3" s="4"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="8">
         <v>97</v>
       </c>
       <c r="B4" s="1">
@@ -6200,7 +6276,7 @@
       <c r="AN4" s="4"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>98</v>
       </c>
       <c r="B5" s="3">
@@ -6246,7 +6322,7 @@
       <c r="AN5" s="4"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="8">
         <v>99</v>
       </c>
       <c r="B6" s="1">
@@ -6292,7 +6368,7 @@
       <c r="AN6" s="4"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -6338,7 +6414,7 @@
       <c r="AN7" s="4"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1">
@@ -6384,7 +6460,7 @@
       <c r="AN8" s="4"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
@@ -6430,7 +6506,7 @@
       <c r="AN9" s="4"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1">
@@ -6476,7 +6552,7 @@
       <c r="AN10" s="4"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3">
@@ -6522,7 +6598,7 @@
       <c r="AN11" s="4"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -6568,7 +6644,7 @@
       <c r="AN12" s="4"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3">
@@ -6614,7 +6690,7 @@
       <c r="AN13" s="4"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1">
@@ -6660,7 +6736,7 @@
       <c r="AN14" s="4"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="3">
@@ -6706,7 +6782,7 @@
       <c r="AN15" s="4"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1">
@@ -6752,7 +6828,7 @@
       <c r="AN16" s="4"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <v>10</v>
       </c>
       <c r="B17" s="3">
@@ -6798,7 +6874,7 @@
       <c r="AN17" s="4"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="8">
         <v>11</v>
       </c>
       <c r="B18" s="1">
@@ -6844,7 +6920,7 @@
       <c r="AN18" s="4"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <v>12</v>
       </c>
       <c r="B19" s="3">
@@ -6890,7 +6966,7 @@
       <c r="AN19" s="4"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="8">
         <v>13</v>
       </c>
       <c r="B20" s="1">
@@ -6936,7 +7012,7 @@
       <c r="AN20" s="4"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="7">
         <v>14</v>
       </c>
       <c r="B21" s="3">
@@ -6982,7 +7058,7 @@
       <c r="AN21" s="4"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="8">
         <v>15</v>
       </c>
       <c r="B22" s="1">
@@ -7028,7 +7104,7 @@
       <c r="AN22" s="4"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="7">
         <v>16</v>
       </c>
       <c r="B23" s="3">
@@ -7074,7 +7150,7 @@
       <c r="AN23" s="4"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="8">
         <v>17</v>
       </c>
       <c r="B24" s="1">
@@ -7120,7 +7196,7 @@
       <c r="AN24" s="4"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="7">
         <v>18</v>
       </c>
       <c r="B25" s="3">
@@ -7166,7 +7242,7 @@
       <c r="AN25" s="4"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="8">
         <v>19</v>
       </c>
       <c r="B26" s="1">
@@ -7212,7 +7288,7 @@
       <c r="AN26" s="4"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>20</v>
       </c>
       <c r="B27" s="3">
@@ -7258,7 +7334,7 @@
       <c r="AN27" s="4"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="8">
         <v>21</v>
       </c>
       <c r="B28" s="1">
@@ -7304,14 +7380,16 @@
       <c r="AN28" s="4"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="7">
         <v>22</v>
       </c>
       <c r="B29" s="3">
         <v>426467985.50999999</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -7350,14 +7428,16 @@
       <c r="AN29" s="4"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="7">
         <v>23</v>
       </c>
       <c r="B30" s="3">
         <v>471856109.18874192</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -7396,8 +7476,12 @@
       <c r="AN30" s="4"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="11">
+        <v>505920158.7602604</v>
+      </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -7438,8 +7522,12 @@
       <c r="AN31" s="4"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="11">
+        <v>219609763.67566624</v>
+      </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -7481,7 +7569,7 @@
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="5"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -7523,7 +7611,7 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="5"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -7565,7 +7653,7 @@
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="5"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -7607,7 +7695,7 @@
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="5"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -7649,7 +7737,7 @@
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -7691,7 +7779,7 @@
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="5"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -7733,7 +7821,7 @@
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="5"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -7775,7 +7863,7 @@
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="5"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -7817,7 +7905,7 @@
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="5"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -7859,7 +7947,7 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="5"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -7901,7 +7989,7 @@
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="5"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -7943,7 +8031,7 @@
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="5"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="5"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -7985,7 +8073,7 @@
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="5"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -8037,8 +8125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FC553E-21A9-468B-964D-897B06F43937}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Replaced refund report with latest report (#901)
</commit_message>
<xml_diff>
--- a/public/files/refund-report.xlsx
+++ b/public/files/refund-report.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JaimeLHabersat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSA Data\Reports\Refund Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56B669C-97F0-43E5-9512-84E5027E9F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AC2405-6001-4E38-AEDB-2BA0A1F207E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{59F6B7B8-CB1F-4012-B8AB-951C4865ED6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{59F6B7B8-CB1F-4012-B8AB-951C4865ED6A}"/>
   </bookViews>
   <sheets>
-    <sheet name="GSA SmartPay Net Refunds" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="GSA SmartPay Net Refunds Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="GSA SmartPay Net Refunds" sheetId="1" r:id="rId1"/>
+    <sheet name="GSA SmartPay Net Refunds Chart" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>09</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25*</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>FY25 is through 3/31/2025.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -160,12 +172,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -226,7 +239,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="1"/>
-              <a:t>GSA SmartPay Net Refunds</a:t>
+              <a:t>GSA SmartPay(R) Net Refunds</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -293,7 +306,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
             <a:ln w="111125">
               <a:solidFill>
@@ -312,7 +325,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -338,7 +351,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -364,7 +377,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -390,7 +403,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -416,7 +429,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -442,7 +455,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -468,7 +481,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -494,7 +507,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -520,7 +533,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -546,7 +559,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -572,7 +585,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -598,7 +611,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -624,7 +637,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -648,7 +661,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -672,7 +685,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -696,7 +709,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -720,7 +733,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -744,7 +757,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -768,7 +781,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -792,7 +805,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -816,7 +829,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -840,7 +853,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -864,7 +877,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -891,7 +904,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -918,7 +931,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -972,10 +985,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="111125">
                 <a:solidFill>
@@ -993,6 +1003,60 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000034-4997-45EA-ACF8-DAC8DB9AF015}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="111125">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000036-01FC-4C42-9561-839368366CD4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="111125">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-01FC-4C42-9561-839368366CD4}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1020,7 +1084,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1069,7 +1133,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1118,7 +1182,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1167,7 +1231,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -1208,7 +1272,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -1250,9 +1314,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'GSA SmartPay Net Refunds'!$A$4:$A$30</c:f>
+              <c:f>'GSA SmartPay Net Refunds'!$A$4:$A$32</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>97</c:v>
                 </c:pt>
@@ -1333,16 +1397,22 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>25*</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'GSA SmartPay Net Refunds'!$B$4:$B$30</c:f>
+              <c:f>'GSA SmartPay Net Refunds'!$B$4:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>6000000</c:v>
                 </c:pt>
@@ -1423,6 +1493,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>471856109.18874192</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>505920158.7602604</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>219609763.67566624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1461,7 +1537,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1493,7 +1569,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1531,7 +1607,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1567,7 +1643,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1580,7 +1656,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Dollars </a:t>
                 </a:r>
               </a:p>
@@ -1599,7 +1675,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1631,7 +1707,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4739,7 +4815,7 @@
       <cdr:y>0.89885</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38472</cdr:x>
+      <cdr:x>0.39841</cdr:x>
       <cdr:y>0.94336</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -4755,8 +4831,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2114551" y="4232138"/>
-          <a:ext cx="828675" cy="209550"/>
+          <a:off x="2114567" y="4232135"/>
+          <a:ext cx="933433" cy="209553"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4767,7 +4843,7 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>SmartPay</a:t>
           </a:r>
           <a:r>
@@ -4785,8 +4861,8 @@
       <cdr:y>0.89686</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.64534</cdr:x>
-      <cdr:y>0.94136</cdr:y>
+      <cdr:x>0.65115</cdr:x>
+      <cdr:y>0.95954</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4801,8 +4877,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4108450" y="4222750"/>
-          <a:ext cx="828675" cy="209550"/>
+          <a:off x="4108412" y="4222765"/>
+          <a:ext cx="873164" cy="295123"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4877,11 +4953,11 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>SmartPay</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
             <a:t> 2</a:t>
           </a:r>
         </a:p>
@@ -4894,8 +4970,8 @@
       <cdr:y>0.89686</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.86198</cdr:x>
-      <cdr:y>0.94136</cdr:y>
+      <cdr:x>0.88148</cdr:x>
+      <cdr:y>0.95145</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4910,8 +4986,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5765800" y="4222750"/>
-          <a:ext cx="828675" cy="209550"/>
+          <a:off x="5765793" y="4222765"/>
+          <a:ext cx="977908" cy="257023"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4986,7 +5062,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>SmartPay</a:t>
           </a:r>
           <a:r>
@@ -6012,19 +6088,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F221688A-C4CC-471D-9445-3D65F494C309}">
   <dimension ref="A1:AN45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
+      <c r="A1" s="7"/>
       <c r="B1" s="2"/>
       <c r="C1" s="5"/>
       <c r="D1" s="4"/>
@@ -6066,7 +6142,7 @@
       <c r="AN1" s="4"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2"/>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
@@ -6108,7 +6184,7 @@
       <c r="AN2" s="4"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -6154,7 +6230,7 @@
       <c r="AN3" s="4"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="8">
         <v>97</v>
       </c>
       <c r="B4" s="1">
@@ -6200,7 +6276,7 @@
       <c r="AN4" s="4"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>98</v>
       </c>
       <c r="B5" s="3">
@@ -6246,7 +6322,7 @@
       <c r="AN5" s="4"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="8">
         <v>99</v>
       </c>
       <c r="B6" s="1">
@@ -6292,7 +6368,7 @@
       <c r="AN6" s="4"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -6338,7 +6414,7 @@
       <c r="AN7" s="4"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1">
@@ -6384,7 +6460,7 @@
       <c r="AN8" s="4"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
@@ -6430,7 +6506,7 @@
       <c r="AN9" s="4"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1">
@@ -6476,7 +6552,7 @@
       <c r="AN10" s="4"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3">
@@ -6522,7 +6598,7 @@
       <c r="AN11" s="4"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -6568,7 +6644,7 @@
       <c r="AN12" s="4"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3">
@@ -6614,7 +6690,7 @@
       <c r="AN13" s="4"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1">
@@ -6660,7 +6736,7 @@
       <c r="AN14" s="4"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="3">
@@ -6706,7 +6782,7 @@
       <c r="AN15" s="4"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1">
@@ -6752,7 +6828,7 @@
       <c r="AN16" s="4"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <v>10</v>
       </c>
       <c r="B17" s="3">
@@ -6798,7 +6874,7 @@
       <c r="AN17" s="4"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="8">
         <v>11</v>
       </c>
       <c r="B18" s="1">
@@ -6844,7 +6920,7 @@
       <c r="AN18" s="4"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <v>12</v>
       </c>
       <c r="B19" s="3">
@@ -6890,7 +6966,7 @@
       <c r="AN19" s="4"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="8">
         <v>13</v>
       </c>
       <c r="B20" s="1">
@@ -6936,7 +7012,7 @@
       <c r="AN20" s="4"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="7">
         <v>14</v>
       </c>
       <c r="B21" s="3">
@@ -6982,7 +7058,7 @@
       <c r="AN21" s="4"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="8">
         <v>15</v>
       </c>
       <c r="B22" s="1">
@@ -7028,7 +7104,7 @@
       <c r="AN22" s="4"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="7">
         <v>16</v>
       </c>
       <c r="B23" s="3">
@@ -7074,7 +7150,7 @@
       <c r="AN23" s="4"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="8">
         <v>17</v>
       </c>
       <c r="B24" s="1">
@@ -7120,7 +7196,7 @@
       <c r="AN24" s="4"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="7">
         <v>18</v>
       </c>
       <c r="B25" s="3">
@@ -7166,7 +7242,7 @@
       <c r="AN25" s="4"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="8">
         <v>19</v>
       </c>
       <c r="B26" s="1">
@@ -7212,7 +7288,7 @@
       <c r="AN26" s="4"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>20</v>
       </c>
       <c r="B27" s="3">
@@ -7258,7 +7334,7 @@
       <c r="AN27" s="4"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="8">
         <v>21</v>
       </c>
       <c r="B28" s="1">
@@ -7304,14 +7380,16 @@
       <c r="AN28" s="4"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="7">
         <v>22</v>
       </c>
       <c r="B29" s="3">
         <v>426467985.50999999</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -7350,14 +7428,16 @@
       <c r="AN29" s="4"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="7">
         <v>23</v>
       </c>
       <c r="B30" s="3">
         <v>471856109.18874192</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -7396,8 +7476,12 @@
       <c r="AN30" s="4"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="11">
+        <v>505920158.7602604</v>
+      </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -7438,8 +7522,12 @@
       <c r="AN31" s="4"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="11">
+        <v>219609763.67566624</v>
+      </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -7481,7 +7569,7 @@
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="5"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -7523,7 +7611,7 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="5"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -7565,7 +7653,7 @@
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="5"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -7607,7 +7695,7 @@
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="5"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -7649,7 +7737,7 @@
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -7691,7 +7779,7 @@
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="5"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -7733,7 +7821,7 @@
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="5"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -7775,7 +7863,7 @@
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="5"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -7817,7 +7905,7 @@
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="5"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -7859,7 +7947,7 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="5"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -7901,7 +7989,7 @@
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="5"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -7943,7 +8031,7 @@
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="5"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="5"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -7985,7 +8073,7 @@
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="5"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -8037,8 +8125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FC553E-21A9-468B-964D-897B06F43937}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>